<commit_message>
Texturen überarbeitet und Kodierung vereinheitlicht
fix #33
</commit_message>
<xml_diff>
--- a/Powerpoint_Slides.xlsx
+++ b/Powerpoint_Slides.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OMSI\Projekte\Nuntius_FIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A058D24-4B2A-478B-AE2B-032BA3BC4C4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7065F71E-758B-4A9B-AC71-D788F26A1EA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{734FB089-A332-43BE-BC40-32647E471D5B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Announcements_BusstopAnnouncementsOff.dds</t>
   </si>
@@ -109,6 +109,21 @@
   </si>
   <si>
     <t>Welcome.dds</t>
+  </si>
+  <si>
+    <t>Menu_Apperance_ThemeAuto.dds</t>
+  </si>
+  <si>
+    <t>Menu_Apperance_ThemeManual.dds</t>
+  </si>
+  <si>
+    <t>Menu_Info.dds</t>
+  </si>
+  <si>
+    <t>Menu_Device.dds</t>
+  </si>
+  <si>
+    <t>Menu_Misc.dds</t>
   </si>
 </sst>
 </file>
@@ -460,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F35E60B6-81FC-4EFE-9DDD-58C5FBDBE829}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,6 +707,46 @@
         <v>25</v>
       </c>
     </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A1:B28">
     <sortCondition ref="A1:A28"/>

</xml_diff>